<commit_message>
fixes for working hrs constraint
</commit_message>
<xml_diff>
--- a/scheduler/data/PolishingOrders.xlsx
+++ b/scheduler/data/PolishingOrders.xlsx
@@ -581,7 +581,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E324"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E2" s="5">
         <v>43344.382638888892</v>
@@ -650,7 +650,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E3" s="5">
         <v>43344.383333333331</v>
@@ -667,7 +667,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E4" s="5">
         <v>43344.573611111111</v>
@@ -684,7 +684,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E5" s="5">
         <v>43349.256944444445</v>
@@ -701,7 +701,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E6" s="5">
         <v>43349.619444444441</v>
@@ -718,7 +718,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E7" s="5">
         <v>43350.333333333336</v>
@@ -735,7 +735,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E8" s="5">
         <v>43350.387499999997</v>
@@ -752,7 +752,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E9" s="5">
         <v>43350.40902777778</v>
@@ -769,7 +769,7 @@
         <v>23</v>
       </c>
       <c r="D10" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E10" s="5">
         <v>43350.436111111114</v>
@@ -786,7 +786,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="3">
-        <v>35</v>
+        <v>35000</v>
       </c>
       <c r="E11" s="5">
         <v>43350.457638888889</v>
@@ -803,7 +803,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E12" s="5">
         <v>43350.541666666664</v>
@@ -820,7 +820,7 @@
         <v>29</v>
       </c>
       <c r="D13" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E13" s="5">
         <v>43350.541666666664</v>
@@ -837,7 +837,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="3">
-        <v>35</v>
+        <v>35000</v>
       </c>
       <c r="E14" s="5">
         <v>43350.587500000001</v>
@@ -854,7 +854,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E15" s="5">
         <v>43350.613888888889</v>
@@ -871,7 +871,7 @@
         <v>33</v>
       </c>
       <c r="D16" s="3">
-        <v>35</v>
+        <v>35000</v>
       </c>
       <c r="E16" s="5">
         <v>43351.585416666669</v>
@@ -888,7 +888,7 @@
         <v>37</v>
       </c>
       <c r="D17" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E17" s="5">
         <v>43352.314583333333</v>
@@ -905,7 +905,7 @@
         <v>39</v>
       </c>
       <c r="D18" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E18" s="5">
         <v>43355.572916666664</v>
@@ -922,7 +922,7 @@
         <v>41</v>
       </c>
       <c r="D19" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E19" s="5">
         <v>43355.693749999999</v>
@@ -939,7 +939,7 @@
         <v>41</v>
       </c>
       <c r="D20" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E20" s="5">
         <v>43355.779166666667</v>
@@ -956,7 +956,7 @@
         <v>43</v>
       </c>
       <c r="D21" s="3">
-        <v>35</v>
+        <v>35000</v>
       </c>
       <c r="E21" s="5">
         <v>43356.720833333333</v>
@@ -973,7 +973,7 @@
         <v>46</v>
       </c>
       <c r="D22" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E22" s="5">
         <v>43357.333333333336</v>
@@ -990,7 +990,7 @@
         <v>17</v>
       </c>
       <c r="D23" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E23" s="5">
         <v>43357.541666666664</v>
@@ -1007,7 +1007,7 @@
         <v>48</v>
       </c>
       <c r="D24" s="3">
-        <v>35</v>
+        <v>35000</v>
       </c>
       <c r="E24" s="5">
         <v>43357.779166666667</v>
@@ -1024,7 +1024,7 @@
         <v>50</v>
       </c>
       <c r="D25" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E25" s="5">
         <v>43359.541666666664</v>
@@ -1041,7 +1041,7 @@
         <v>7</v>
       </c>
       <c r="D26" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E26" s="5">
         <v>43359.770833333336</v>
@@ -1058,7 +1058,7 @@
         <v>35</v>
       </c>
       <c r="D27" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E27" s="5">
         <v>43362.333333333336</v>
@@ -1075,7 +1075,7 @@
         <v>16</v>
       </c>
       <c r="D28" s="3">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="E28" s="5">
         <v>43362.6875</v>

</xml_diff>

<commit_message>
fixed schedule break down and handle weekends
</commit_message>
<xml_diff>
--- a/scheduler/data/PolishingOrders.xlsx
+++ b/scheduler/data/PolishingOrders.xlsx
@@ -581,7 +581,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E2" s="5">
         <v>43344.382638888892</v>
@@ -650,7 +650,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E3" s="5">
         <v>43344.383333333331</v>
@@ -667,7 +667,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E4" s="5">
         <v>43344.573611111111</v>
@@ -684,7 +684,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E5" s="5">
         <v>43349.256944444445</v>
@@ -701,7 +701,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E6" s="5">
         <v>43349.619444444441</v>
@@ -718,7 +718,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E7" s="5">
         <v>43350.333333333336</v>
@@ -735,7 +735,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E8" s="5">
         <v>43350.387499999997</v>
@@ -752,7 +752,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E9" s="5">
         <v>43350.40902777778</v>
@@ -769,7 +769,7 @@
         <v>23</v>
       </c>
       <c r="D10" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E10" s="5">
         <v>43350.436111111114</v>
@@ -786,7 +786,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="3">
-        <v>35000</v>
+        <v>350</v>
       </c>
       <c r="E11" s="5">
         <v>43350.457638888889</v>
@@ -803,7 +803,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E12" s="5">
         <v>43350.541666666664</v>
@@ -820,7 +820,7 @@
         <v>29</v>
       </c>
       <c r="D13" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E13" s="5">
         <v>43350.541666666664</v>
@@ -837,7 +837,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="3">
-        <v>35000</v>
+        <v>3500</v>
       </c>
       <c r="E14" s="5">
         <v>43350.587500000001</v>
@@ -871,7 +871,7 @@
         <v>33</v>
       </c>
       <c r="D16" s="3">
-        <v>35000</v>
+        <v>3500</v>
       </c>
       <c r="E16" s="5">
         <v>43351.585416666669</v>
@@ -888,7 +888,7 @@
         <v>37</v>
       </c>
       <c r="D17" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E17" s="5">
         <v>43352.314583333333</v>
@@ -905,7 +905,7 @@
         <v>39</v>
       </c>
       <c r="D18" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E18" s="5">
         <v>43355.572916666664</v>
@@ -922,7 +922,7 @@
         <v>41</v>
       </c>
       <c r="D19" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E19" s="5">
         <v>43355.693749999999</v>
@@ -939,7 +939,7 @@
         <v>41</v>
       </c>
       <c r="D20" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E20" s="5">
         <v>43355.779166666667</v>
@@ -956,7 +956,7 @@
         <v>43</v>
       </c>
       <c r="D21" s="3">
-        <v>35000</v>
+        <v>350</v>
       </c>
       <c r="E21" s="5">
         <v>43356.720833333333</v>
@@ -973,7 +973,7 @@
         <v>46</v>
       </c>
       <c r="D22" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E22" s="5">
         <v>43357.333333333336</v>
@@ -990,7 +990,7 @@
         <v>17</v>
       </c>
       <c r="D23" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E23" s="5">
         <v>43357.541666666664</v>
@@ -1007,7 +1007,7 @@
         <v>48</v>
       </c>
       <c r="D24" s="3">
-        <v>35000</v>
+        <v>350</v>
       </c>
       <c r="E24" s="5">
         <v>43357.779166666667</v>
@@ -1024,7 +1024,7 @@
         <v>50</v>
       </c>
       <c r="D25" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E25" s="5">
         <v>43359.541666666664</v>
@@ -1041,7 +1041,7 @@
         <v>7</v>
       </c>
       <c r="D26" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E26" s="5">
         <v>43359.770833333336</v>
@@ -1058,7 +1058,7 @@
         <v>35</v>
       </c>
       <c r="D27" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E27" s="5">
         <v>43362.333333333336</v>
@@ -1075,7 +1075,7 @@
         <v>16</v>
       </c>
       <c r="D28" s="3">
-        <v>3500</v>
+        <v>350</v>
       </c>
       <c r="E28" s="5">
         <v>43362.6875</v>

</xml_diff>